<commit_message>
updated with modifications on 07/31
</commit_message>
<xml_diff>
--- a/DB-design/fields-to-consider.xlsx
+++ b/DB-design/fields-to-consider.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Asit\Personal\Berkley BootCamp\Module-20 Project\nba-player-analytics\DB-design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBF2983-00E1-45AE-ADD8-9564511F43A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45843AF9-B369-4EBA-9E0A-5A7CFA8E7CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{78AE7BCC-BD40-4637-8F60-941A91954F9A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{78AE7BCC-BD40-4637-8F60-941A91954F9A}"/>
   </bookViews>
   <sheets>
     <sheet name="final_data" sheetId="1" r:id="rId1"/>
     <sheet name="PLAYERS_D" sheetId="2" r:id="rId2"/>
     <sheet name="PLAYERS_STATS_F" sheetId="3" r:id="rId3"/>
     <sheet name="PLAYERS_SALARY_F" sheetId="4" r:id="rId4"/>
+    <sheet name="PLAYERS_CATEGORY" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="25">
   <si>
     <t>player_id</t>
   </si>
@@ -108,7 +109,10 @@
     <t>pk</t>
   </si>
   <si>
-    <t>fk</t>
+    <t>category</t>
+  </si>
+  <si>
+    <t>fk (PLAYERS_D.player_id)</t>
   </si>
 </sst>
 </file>
@@ -1104,9 +1108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEEC03A6-9752-44DA-AAD7-8FBA030D8601}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1216,8 +1218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EFEF06-3724-4713-97B3-6F166787D5D5}">
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1756,7 +1758,7 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1768,7 +1770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCC8C3E-D1A5-430A-9D16-8A74685EDC2B}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -1898,7 +1900,40 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB64304-A3C4-4480-BACC-E4620A1E7BF8}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>